<commit_message>
add RC filter to string in telem, regenerate outputs
</commit_message>
<xml_diff>
--- a/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
+++ b/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\Project Outputs for mppt\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B5ACB96-9E46-4172-948E-4D92FBB57829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2529AB02-138E-4E9A-A856-21F19A9DB2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{70CB24EF-95FE-465F-9ABE-0163A17CE624}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{50C1E56D-9D7C-425C-935E-DA28E1F4EDD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-mppt" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
     <t>Cap Ceramic 0.1uF 250V X7T 10% SMD 0805 125°C Blister Plastic T/R</t>
   </si>
   <si>
-    <t>C6, C8, C10, C11, C12, C17, C18, C27, C35, C37, C39, C45, C47, C49, C50, C51, C52, C54, C55, C56, C58, C59, C60, C65, C66</t>
+    <t>C6, C8, C10, C11, C12, C17, C18, C27, C35, C37, C39, C45, C47, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C65, C66, C67, C68, C69</t>
   </si>
   <si>
     <t>SMD-0805C</t>
@@ -120,7 +120,7 @@
     <t>CAPAE110103X126M</t>
   </si>
   <si>
-    <t>C20, C26, C53, C57, C61</t>
+    <t>C20, C26</t>
   </si>
   <si>
     <t>B340A-13-F</t>
@@ -288,6 +288,21 @@
     <t>PMR18EZPFV4L00</t>
   </si>
   <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R2, R23, R31, R40, R43, R46</t>
+  </si>
+  <si>
+    <t>SMD-0805-RES</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ102V</t>
+  </si>
+  <si>
     <t>100k</t>
   </si>
   <si>
@@ -297,9 +312,6 @@
     <t>R3, R9, R24, R32</t>
   </si>
   <si>
-    <t>SMD-0805-RES</t>
-  </si>
-  <si>
     <t>ERJ-6ENF1003V</t>
   </si>
   <si>
@@ -373,18 +385,6 @@
   </si>
   <si>
     <t>ERJ-6ENF3002V</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 5% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R40, R43, R46</t>
-  </si>
-  <si>
-    <t>ERJ-6GEYJ102V</t>
   </si>
   <si>
     <t>NCP21XM472J03RA</t>
@@ -865,7 +865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D880E17C-B8F3-437C-933A-8B353D30D7D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B728756-B257-4E25-AD56-D44F3F0EB7F4}">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -972,7 +972,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="1">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1012,7 +1012,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
         <v>87</v>
       </c>
       <c r="F22" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,7 +1352,7 @@
         <v>95</v>
       </c>
       <c r="F24" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1372,7 +1372,7 @@
         <v>99</v>
       </c>
       <c r="F25" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1392,7 +1392,7 @@
         <v>103</v>
       </c>
       <c r="F26" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1412,7 +1412,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1432,7 +1432,7 @@
         <v>111</v>
       </c>
       <c r="F28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix two more 0.1uf resistors to correct part
</commit_message>
<xml_diff>
--- a/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
+++ b/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\Project Outputs for mppt\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2529AB02-138E-4E9A-A856-21F19A9DB2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B56F5FB-D026-4297-ACE1-2B7EEB38793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{50C1E56D-9D7C-425C-935E-DA28E1F4EDD1}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{F11C0C1D-81F0-4A74-B0E3-1A4B2800B286}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-mppt" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t>Comment</t>
   </si>
@@ -99,7 +99,7 @@
     <t>Cap Ceramic 0.1uF 250V X7T 10% SMD 0805 125°C Blister Plastic T/R</t>
   </si>
   <si>
-    <t>C6, C8, C10, C11, C12, C17, C18, C27, C35, C37, C39, C45, C47, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C65, C66, C67, C68, C69</t>
+    <t>C6, C8, C10, C11, C12, C17, C18, C20, C26, C27, C35, C37, C39, C45, C47, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C65, C66, C67, C68, C69</t>
   </si>
   <si>
     <t>SMD-0805C</t>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>CAPAE110103X126M</t>
-  </si>
-  <si>
-    <t>C20, C26</t>
   </si>
   <si>
     <t>B340A-13-F</t>
@@ -865,8 +862,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B728756-B257-4E25-AD56-D44F3F0EB7F4}">
-  <dimension ref="A1:F39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A105DFD-3CC1-48A3-AC74-46CB720F9F6F}">
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -972,7 +969,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,99 +994,99 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F11" s="1">
         <v>3</v>
@@ -1097,59 +1094,59 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F14" s="1">
         <v>4</v>
@@ -1157,119 +1154,119 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="F17" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F18" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="F19" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F20" s="1">
         <v>3</v>
@@ -1277,59 +1274,59 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F21" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F22" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F23" s="1">
         <v>4</v>
@@ -1337,116 +1334,116 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F25" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F26" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>115</v>
@@ -1457,99 +1454,99 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F30" s="1">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F31" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="F32" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="F33" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -1557,19 +1554,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
@@ -1577,19 +1574,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
@@ -1597,19 +1594,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
@@ -1617,41 +1614,21 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F39" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add boms to output for ordering, including one from digikey
</commit_message>
<xml_diff>
--- a/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
+++ b/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\solar_car_hardware\mppt\Project Outputs for mppt\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B56F5FB-D026-4297-ACE1-2B7EEB38793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB0F453E-253D-46B7-B459-99D6A2C07C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{F11C0C1D-81F0-4A74-B0E3-1A4B2800B286}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{B586560E-407B-40C8-9FA9-975BA26FE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-mppt" sheetId="1" r:id="rId1"/>
@@ -862,7 +862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A105DFD-3CC1-48A3-AC74-46CB720F9F6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD3C7B-2C47-4C67-8F69-34E2AE62F69F}">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
add new gerber outputs
</commit_message>
<xml_diff>
--- a/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
+++ b/mppt/Project Outputs for mppt/BOM/Bill of Materials-mppt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19202\Desktop\badgerloop\git_repos\solar_car_hardware\mppt\Project Outputs for mppt\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{842B38E5-7372-4C4E-9BAA-A17CDEC97C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C89E2F1-506E-4039-B7DE-97F5506A2A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{F93E6DA5-1C97-4941-9E79-7F25B30BBC1C}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{7E25BE3D-78B2-4122-A60B-B923D0510803}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-mppt" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
     <t>RES SMD 100K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>R3, R10, R16, R24, R29, R32</t>
+    <t>R3, R10, R16, R24, R29, R32, R65</t>
   </si>
   <si>
     <t>ERJ-6ENF1003V</t>
@@ -1013,7 +1013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E970304E-898E-4DE3-9362-FF827713F849}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3D8988-9576-40B7-B0DF-4961055E1EFA}">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1580,7 +1580,7 @@
         <v>112</v>
       </c>
       <c r="F28" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>